<commit_message>
view data of 240525
</commit_message>
<xml_diff>
--- a/Sensoren/sensoren.xlsx
+++ b/Sensoren/sensoren.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Janjo/Documents/MEINE DOKUMENTE/switchDrive/Private/Kaltluft/Sensoren/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Janjo/Documents/MEINE_DOKUMENTE/Projects/kaltluftstrom/Sensoren/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A0F983-472C-B64D-9284-1E9943803A6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1784A5D-7BE0-E848-9CC9-C2A92BE6E78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="1" xr2:uid="{A79CE484-3A61-7749-AAC4-367793E8D5A1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19700" activeTab="1" xr2:uid="{A79CE484-3A61-7749-AAC4-367793E8D5A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Gruppen" sheetId="2" r:id="rId1"/>
@@ -20,17 +20,28 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">WTDL1!$A$1:$M$1</definedName>
     <definedName name="groups">Gruppen!$A$2:$C$9</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="119">
   <si>
     <t>ID</t>
   </si>
@@ -221,9 +232,6 @@
     <t>Speicherfehler. Messungen konnten grösstenteils wiederhergestellt werden</t>
   </si>
   <si>
-    <t>Position nicht eindeutig definierbar.</t>
-  </si>
-  <si>
     <t>H in Schneise 2</t>
   </si>
   <si>
@@ -305,9 +313,6 @@
     <t>SEQ3471215</t>
   </si>
   <si>
-    <t>Erschlagen bei Holzschlag. Daten konnten bis 14.12.22 wiederhergestellt werden. Sensor noch einwandfrei.</t>
-  </si>
-  <si>
     <t>W42.2</t>
   </si>
   <si>
@@ -333,6 +338,66 @@
   </si>
   <si>
     <t>Waldrand unterhalb Forsteingriff</t>
+  </si>
+  <si>
+    <t>W2.3</t>
+  </si>
+  <si>
+    <t>Sensor verschwunden (bemerkt bei Auslesung 25.05.24)</t>
+  </si>
+  <si>
+    <t>SEQ3471207</t>
+  </si>
+  <si>
+    <t>W42.3</t>
+  </si>
+  <si>
+    <t>neu als W11.3 eingesetzt</t>
+  </si>
+  <si>
+    <t>neu als W42.3 eingesetzt</t>
+  </si>
+  <si>
+    <t>W44.2</t>
+  </si>
+  <si>
+    <t>SEQ3471241</t>
+  </si>
+  <si>
+    <t>W11.3</t>
+  </si>
+  <si>
+    <t>Deckel aufgebissen. Daten teilweise wiederhergestellt.</t>
+  </si>
+  <si>
+    <t>Deckel aufgebissen. Datenverlust.</t>
+  </si>
+  <si>
+    <t>vorher als W35.1 im Einsatz</t>
+  </si>
+  <si>
+    <t>Vorher als W35.2 im Einsatz</t>
+  </si>
+  <si>
+    <t>W4.2</t>
+  </si>
+  <si>
+    <t>UEQ2351805</t>
+  </si>
+  <si>
+    <t>Erschlagen bei Holzschlag. Daten konnten bis 14.12.22 wiederhergestellt werden. Sensor noch einwandfrei. Sensor hat am 25.5.24 gefehlt.</t>
+  </si>
+  <si>
+    <t>Gruppenzugehörigkeit nicht eindeutig definierbar.</t>
+  </si>
+  <si>
+    <t>UEQ2351794</t>
+  </si>
+  <si>
+    <t>UEQ2351795</t>
+  </si>
+  <si>
+    <t>UEQ2351810</t>
   </si>
 </sst>
 </file>
@@ -415,9 +480,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -455,7 +520,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -561,7 +626,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -703,7 +768,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -833,13 +898,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,7 +961,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -910,7 +975,7 @@
         <v>Waldrand</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H2" s="2">
         <v>44747</v>
@@ -924,7 +989,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -958,7 +1023,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -972,7 +1037,7 @@
         <v>Waldrand</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H4" s="2">
         <v>44747</v>
@@ -986,7 +1051,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -1000,7 +1065,7 @@
         <v>Waldrand</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H5" s="2">
         <v>44747</v>
@@ -1008,9 +1073,14 @@
       <c r="I5" s="2">
         <v>44748</v>
       </c>
-      <c r="J5" s="2"/>
+      <c r="J5" s="2">
+        <v>45437</v>
+      </c>
+      <c r="K5" t="s">
+        <v>112</v>
+      </c>
       <c r="M5" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1018,7 +1088,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -1032,7 +1102,7 @@
         <v>Waldrand</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H6" s="2">
         <v>44747</v>
@@ -1052,7 +1122,7 @@
         <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H7" s="2">
         <v>44747</v>
@@ -1061,7 +1131,7 @@
         <v>44748</v>
       </c>
       <c r="M7" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1083,7 +1153,7 @@
         <v>Referenz</v>
       </c>
       <c r="F8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H8" s="2">
         <v>44747</v>
@@ -1122,7 +1192,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -1136,7 +1206,7 @@
         <v>Wald</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H10" s="2">
         <v>44747</v>
@@ -1164,7 +1234,7 @@
         <v>Quartier</v>
       </c>
       <c r="F11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J11" s="2">
         <v>45154</v>
@@ -1175,7 +1245,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
@@ -1189,7 +1259,7 @@
         <v>Quartier</v>
       </c>
       <c r="F12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1211,7 +1281,7 @@
         <v>Wald</v>
       </c>
       <c r="F13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1233,15 +1303,15 @@
         <v>Wald</v>
       </c>
       <c r="F14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -1255,7 +1325,10 @@
         <v>Wald</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="M15" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1263,7 +1336,7 @@
         <v>32</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -1277,15 +1350,18 @@
         <v>Wald</v>
       </c>
       <c r="F16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="M16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
@@ -1299,15 +1375,15 @@
         <v>Holzschlag</v>
       </c>
       <c r="F17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
         <v>34</v>
@@ -1321,18 +1397,18 @@
         <v>Holzschlag</v>
       </c>
       <c r="F18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
         <v>34</v>
@@ -1346,15 +1422,15 @@
         <v>Holzschlag</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s">
         <v>34</v>
@@ -1368,15 +1444,24 @@
         <v>Holzschlag</v>
       </c>
       <c r="F20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="J20" s="2">
+        <v>45437</v>
+      </c>
+      <c r="K20" t="s">
+        <v>105</v>
+      </c>
+      <c r="M20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C21" t="s">
         <v>34</v>
@@ -1390,10 +1475,10 @@
         <v>Holzschlag</v>
       </c>
       <c r="F21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>39</v>
       </c>
@@ -1412,10 +1497,10 @@
         <v>Bach</v>
       </c>
       <c r="F22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>42</v>
       </c>
@@ -1434,10 +1519,10 @@
         <v>Bach</v>
       </c>
       <c r="F23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -1456,7 +1541,7 @@
         <v>Waldrand</v>
       </c>
       <c r="F24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H24" s="2">
         <v>44913</v>
@@ -1464,13 +1549,22 @@
       <c r="I24" s="2">
         <v>44913</v>
       </c>
+      <c r="J24" s="2">
+        <v>45437</v>
+      </c>
+      <c r="K24" t="s">
+        <v>99</v>
+      </c>
       <c r="L24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
@@ -1487,7 +1581,7 @@
         <v>Quartier</v>
       </c>
       <c r="F25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H25" s="2">
         <v>45154</v>
@@ -1495,13 +1589,25 @@
       <c r="I25" s="2">
         <v>45154</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J25" s="2">
+        <v>45437</v>
+      </c>
+      <c r="K25" t="s">
+        <v>107</v>
+      </c>
+      <c r="L25" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
@@ -1515,10 +1621,193 @@
         <v>Waldrand</v>
       </c>
       <c r="F26" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="J26" s="2">
+        <v>45437</v>
+      </c>
+      <c r="K26" t="s">
+        <v>102</v>
       </c>
       <c r="L26" t="s">
         <v>35</v>
+      </c>
+      <c r="M26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" t="s">
+        <v>101</v>
+      </c>
+      <c r="H27" s="2">
+        <v>45437</v>
+      </c>
+      <c r="I27" s="2">
+        <v>45437</v>
+      </c>
+      <c r="L27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" t="str">
+        <f>VLOOKUP($C28,groups,2)</f>
+        <v>WR</v>
+      </c>
+      <c r="E28" t="str">
+        <f>VLOOKUP($C28,groups,3)</f>
+        <v>Waldrand</v>
+      </c>
+      <c r="F28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H28" s="2">
+        <v>45473</v>
+      </c>
+      <c r="I28" s="2">
+        <v>45474</v>
+      </c>
+      <c r="L28" t="s">
+        <v>90</v>
+      </c>
+      <c r="M28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" ref="D29:D31" si="2">VLOOKUP($C29,groups,2)</f>
+        <v>H</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" ref="E29:E31" si="3">VLOOKUP($C29,groups,3)</f>
+        <v>Holzschlag</v>
+      </c>
+      <c r="F29" t="s">
+        <v>106</v>
+      </c>
+      <c r="H29" s="2">
+        <v>45437</v>
+      </c>
+      <c r="I29" s="2">
+        <v>45437</v>
+      </c>
+      <c r="L29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="2"/>
+        <v>Q</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="3"/>
+        <v>Quartier</v>
+      </c>
+      <c r="F30" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" s="2">
+        <v>45437</v>
+      </c>
+      <c r="I30" s="2">
+        <v>45437</v>
+      </c>
+      <c r="L30" t="s">
+        <v>88</v>
+      </c>
+      <c r="M30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>112</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="2"/>
+        <v>WR</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="3"/>
+        <v>Waldrand</v>
+      </c>
+      <c r="F31" t="s">
+        <v>113</v>
+      </c>
+      <c r="H31" s="2">
+        <v>45473</v>
+      </c>
+      <c r="I31" s="2">
+        <v>45474</v>
+      </c>
+      <c r="L31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>